<commit_message>
Updated Hogan (2008) motif list
</commit_message>
<xml_diff>
--- a/Data/Hogan (2008) top RBP motifs.xlsx
+++ b/Data/Hogan (2008) top RBP motifs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paddyharker/Documents/SENIOR HONOURS/Honours Project 20:21/Results/Motif analysis/Scerevisiae_RBP_motifs_Calbicans/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6EE824-B6D9-334A-80D3-FE1C7D77CB5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9722D0C-6950-3E46-92DA-627CE74CB399}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{D0E74092-547C-1743-8B20-D110A5F4822F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D0E74092-547C-1743-8B20-D110A5F4822F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>RBP</t>
   </si>
@@ -151,13 +151,118 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5'  </t>
+  </si>
+  <si>
+    <t>CDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3'  </t>
+  </si>
+  <si>
+    <t>5'</t>
+  </si>
+  <si>
+    <t>3'</t>
+  </si>
+  <si>
+    <t>Describes whether REFINE or FIRE identified the motif</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>RBPs with an ortholog in Candida albicans which has not been formally named on Candida Gene Order Browser</t>
+  </si>
+  <si>
+    <r>
+      <t>The negative log</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (p-value) of the significance of genome-wide enrichment (based on the hypergeometric distribution) for sequences containing motif sites in targets for 200 bases upstream of start codon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The negative log</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (p-value) of the significance of genome-wide enrichment (based on the hypergeometric distribution) for sequences containing motif sites in targets coding sequences</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The negative log</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (p-value) of the significance of genome-wide enrichment (based on the hypergeometric distribution) for sequences containing motif sites in targets for 200 bases downstream of stop codon</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +281,33 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,10 +333,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,36 +665,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE0C49D-15D1-F14B-907C-C254FBED77F7}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
@@ -557,12 +713,21 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="4">
+        <v>3.4915592250048402</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8.3789437389635193</v>
+      </c>
+      <c r="G2" s="4">
+        <v>163.170369628119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
@@ -571,12 +736,21 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="4">
+        <v>3.09514726532956</v>
+      </c>
+      <c r="F3" s="4">
+        <v>21.783166624484</v>
+      </c>
+      <c r="G3" s="4">
+        <v>88.410528343634098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
@@ -585,12 +759,21 @@
       <c r="D4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="4">
+        <v>5.2829562407298498</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10.904481994055701</v>
+      </c>
+      <c r="G4" s="4">
+        <v>69.359808388638996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C5" t="s">
@@ -599,12 +782,21 @@
       <c r="D5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="4">
+        <v>1.13417442301486</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2.0595064561638901</v>
+      </c>
+      <c r="G5" s="4">
+        <v>58.041443781481597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
@@ -613,12 +805,21 @@
       <c r="D6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="4">
+        <v>1.15178846429084</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4.9661734947507297</v>
+      </c>
+      <c r="G6" s="4">
+        <v>20.535177953545599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C7" t="s">
@@ -627,12 +828,21 @@
       <c r="D7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="4">
+        <v>18.485458116257199</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
@@ -641,12 +851,21 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="4">
+        <v>1.65131980867896</v>
+      </c>
+      <c r="F8" s="4">
+        <v>9.8365439296129803E-40</v>
+      </c>
+      <c r="G8" s="4">
+        <v>16.311121122335202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
@@ -655,12 +874,21 @@
       <c r="D9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="4">
+        <v>2.17398340596058</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3.3184717053976902</v>
+      </c>
+      <c r="G9" s="4">
+        <v>14.711571545988299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C10" t="s">
@@ -669,12 +897,21 @@
       <c r="D10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="4">
+        <v>1.3134441950706</v>
+      </c>
+      <c r="F10" s="4">
+        <v>8.4532144251492003</v>
+      </c>
+      <c r="G10" s="4">
+        <v>12.752079440526501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
@@ -683,12 +920,21 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="E11" s="4">
+        <v>12.517182204657599</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.94466418633481397</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1.0661407051043701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C12" t="s">
@@ -697,12 +943,21 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="4">
+        <v>7.9978931030933103</v>
+      </c>
+      <c r="F12" s="4">
+        <v>11.167071807610199</v>
+      </c>
+      <c r="G12" s="4">
+        <v>6.7919722305269996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C13" t="s">
@@ -711,12 +966,21 @@
       <c r="D13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="4">
+        <v>0.19826468733026401</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.0354816177222399</v>
+      </c>
+      <c r="G13" s="4">
+        <v>10.5483119288859</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C14" t="s">
@@ -725,12 +989,21 @@
       <c r="D14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.0155727397479299</v>
+      </c>
+      <c r="G14" s="4">
+        <v>10.5462322851492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C15" t="s">
@@ -739,12 +1012,21 @@
       <c r="D15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="4">
+        <v>0.95712726050443298</v>
+      </c>
+      <c r="F15" s="4">
+        <v>7.7424626003559004E-5</v>
+      </c>
+      <c r="G15" s="4">
+        <v>10.362807122543799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C16" t="s">
@@ -752,6 +1034,55 @@
       </c>
       <c r="D16" t="s">
         <v>36</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.95438822155606</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1.1191977721339501</v>
+      </c>
+      <c r="G16" s="4">
+        <v>9.9539188775005307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="121" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="104" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="121" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>